<commit_message>
added new behavioral traits to table w/ predictors
</commit_message>
<xml_diff>
--- a/tables/STable4_explanatory_variables.xlsx
+++ b/tables/STable4_explanatory_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/Rutgers/projects/productivity/models/spmodel_tb1/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/Rutgers/projects/productivity/models/sst_productivity/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A2CD9E09-BEFB-8145-926B-CB913D55C825}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0BF249-F51A-6D4D-8444-3AA93E7C3B1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27160" yWindow="780" windowWidth="23040" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7780" yWindow="460" windowWidth="23040" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Source</t>
   </si>
@@ -308,13 +308,52 @@
   </si>
   <si>
     <t>Marine ecoregion</t>
+  </si>
+  <si>
+    <t>Reproductive mode</t>
+  </si>
+  <si>
+    <t>Reproductive guild 1</t>
+  </si>
+  <si>
+    <t>Reproductive guild 2</t>
+  </si>
+  <si>
+    <t>Spawning ground</t>
+  </si>
+  <si>
+    <t>Migratory behavior</t>
+  </si>
+  <si>
+    <t>Spawning frequency</t>
+  </si>
+  <si>
+    <t>Fishbase (finfish, 96%), SeaLifeBase (inverts, 95%)</t>
+  </si>
+  <si>
+    <t>Fishbase (finfish, 91%), SeaLifeBase (inverts, 71%)</t>
+  </si>
+  <si>
+    <t>Fishbase (finfish, 82%), SeaLifeBase (inverts, 67%)</t>
+  </si>
+  <si>
+    <t>Fishbase (finfish, 55%), SeaLifeBase (inverts, 5%)</t>
+  </si>
+  <si>
+    <t>Fishbase (finfish, 62%), SeaLifeBase (inverts, 0%)</t>
+  </si>
+  <si>
+    <t>Fishbase (finfish, 69%), SeaLifeBase (inverts, 0%)</t>
+  </si>
+  <si>
+    <t>Behavioral traits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -352,6 +391,13 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -384,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -397,6 +443,12 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -713,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B29"/>
+  <dimension ref="A2:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -930,7 +982,58 @@
       </c>
     </row>
     <row r="29" spans="1:2">
+      <c r="A29" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>